<commit_message>
feat(FN-1620): update tests for new columns
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Documents\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ukef-my.sharepoint.com/personal/cmccaffery_ukexportfinance_gov_uk/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE6AC15-616B-478F-92A4-0D840031E5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49DFD2CD-4147-4AB1-A87F-4EC839F6174A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -68,41 +68,38 @@
     <t>GBP</t>
   </si>
   <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Facility utilisation</t>
+  </si>
+  <si>
+    <t>Payment currency</t>
+  </si>
+  <si>
     <t>Exporter 2 GEF</t>
   </si>
   <si>
     <t>Exporter 2</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>Fish GEF</t>
-  </si>
-  <si>
-    <t>Fish Exporter</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>Potato GEF</t>
-  </si>
-  <si>
-    <t>Potato Exporter</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Facility utilisation</t>
+    <t>Potato Gef</t>
+  </si>
+  <si>
+    <t>Potato exporter</t>
+  </si>
+  <si>
+    <t>Fees paid to UKEF currency</t>
+  </si>
+  <si>
+    <t>Payment exchange rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +131,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -161,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -178,6 +183,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,23 +498,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -533,8 +544,17 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -559,86 +579,219 @@
       <c r="H2" s="7">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6">
+        <v>600000</v>
+      </c>
+      <c r="F3" s="7">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="7">
+        <v>150</v>
+      </c>
+      <c r="H3" s="7">
+        <v>243</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6">
+        <v>600000</v>
+      </c>
+      <c r="F4" s="7">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="7">
+        <v>45</v>
+      </c>
+      <c r="H4" s="7">
+        <v>45</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4">
-        <v>20001372</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6">
-        <v>300000</v>
-      </c>
-      <c r="F3" s="7">
-        <v>150000</v>
-      </c>
-      <c r="G3" s="7">
-        <v>145</v>
-      </c>
-      <c r="H3" s="7">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4">
-        <v>20001499</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1500000</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1100627.28</v>
-      </c>
-      <c r="G4" s="7">
-        <v>124.75</v>
-      </c>
-      <c r="H4" s="7">
-        <v>976.23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4">
-        <v>20001507</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6">
-        <v>2500000</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1589318.23</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1028.3399999999999</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1028.3399999999999</v>
-      </c>
+      <c r="J4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(FN-1620): Update csv validation for fees paid currency (#2433)
Co-authored-by: Christian McCaffery <cmccaffery@ukexportfinance.gov.uk>
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Documents\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ukef-my.sharepoint.com/personal/cmccaffery_ukexportfinance_gov_uk/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE6AC15-616B-478F-92A4-0D840031E5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49DFD2CD-4147-4AB1-A87F-4EC839F6174A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -68,41 +68,38 @@
     <t>GBP</t>
   </si>
   <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Facility utilisation</t>
+  </si>
+  <si>
+    <t>Payment currency</t>
+  </si>
+  <si>
     <t>Exporter 2 GEF</t>
   </si>
   <si>
     <t>Exporter 2</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>Fish GEF</t>
-  </si>
-  <si>
-    <t>Fish Exporter</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>Potato GEF</t>
-  </si>
-  <si>
-    <t>Potato Exporter</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Facility utilisation</t>
+    <t>Potato Gef</t>
+  </si>
+  <si>
+    <t>Potato exporter</t>
+  </si>
+  <si>
+    <t>Fees paid to UKEF currency</t>
+  </si>
+  <si>
+    <t>Payment exchange rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +131,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -161,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -178,6 +183,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,23 +498,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -533,8 +544,17 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -559,86 +579,219 @@
       <c r="H2" s="7">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6">
+        <v>600000</v>
+      </c>
+      <c r="F3" s="7">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="7">
+        <v>150</v>
+      </c>
+      <c r="H3" s="7">
+        <v>243</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6">
+        <v>600000</v>
+      </c>
+      <c r="F4" s="7">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="7">
+        <v>45</v>
+      </c>
+      <c r="H4" s="7">
+        <v>45</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4">
-        <v>20001372</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6">
-        <v>300000</v>
-      </c>
-      <c r="F3" s="7">
-        <v>150000</v>
-      </c>
-      <c r="G3" s="7">
-        <v>145</v>
-      </c>
-      <c r="H3" s="7">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4">
-        <v>20001499</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1500000</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1100627.28</v>
-      </c>
-      <c r="G4" s="7">
-        <v>124.75</v>
-      </c>
-      <c r="H4" s="7">
-        <v>976.23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4">
-        <v>20001507</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6">
-        <v>2500000</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1589318.23</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1028.3399999999999</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1028.3399999999999</v>
-      </c>
+      <c r="J4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>